<commit_message>
inputs still not working...
</commit_message>
<xml_diff>
--- a/doc/rom_calc_tshoot.xlsx
+++ b/doc/rom_calc_tshoot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aberu\OneDrive\Documents\GitHub\Arcade-TurkeyShoot_MiSTer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E303FE-50D4-4670-A73F-08AA39AB58D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587BAA46-4906-4A4E-95BB-9B83A7516550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROM Map" sheetId="2" r:id="rId1"/>
@@ -711,7 +711,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -865,7 +865,7 @@
         <v>000000000011111111111111</v>
       </c>
       <c r="K4" s="13" t="str">
-        <f t="shared" ref="K4:K26" si="5">DEC2BIN(MOD(QUOTIENT($F4,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F4,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F4,256^0),256),8)</f>
+        <f>DEC2BIN(MOD(QUOTIENT($F4,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F4,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F4,256^0),256),8)</f>
         <v>000000000010000000000000</v>
       </c>
       <c r="L4" s="14" t="s">
@@ -908,7 +908,7 @@
         <v>000000000101111111111111</v>
       </c>
       <c r="K5" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F5,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F5,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F5,256^0),256),8)</f>
         <v>000000000100000000000000</v>
       </c>
       <c r="L5" s="14" t="s">
@@ -951,7 +951,7 @@
         <v>000000000111111111111111</v>
       </c>
       <c r="K6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F6,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F6,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F6,256^0),256),8)</f>
         <v>000000000110000000000000</v>
       </c>
       <c r="L6" s="14" t="s">
@@ -996,7 +996,7 @@
         <v>000000001001111111111111</v>
       </c>
       <c r="K7" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F7,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F7,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F7,256^0),256),8)</f>
         <v>000000001000000000000000</v>
       </c>
       <c r="L7" s="17" t="s">
@@ -1039,7 +1039,7 @@
         <v>000000001011111111111111</v>
       </c>
       <c r="K8" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F8,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F8,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F8,256^0),256),8)</f>
         <v>000000001010000000000000</v>
       </c>
       <c r="L8" s="17" t="s">
@@ -1082,7 +1082,7 @@
         <v>000000001101111111111111</v>
       </c>
       <c r="K9" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F9,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F9,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F9,256^0),256),8)</f>
         <v>000000001100000000000000</v>
       </c>
       <c r="L9" s="17" t="s">
@@ -1125,7 +1125,7 @@
         <v>000000001111111111111111</v>
       </c>
       <c r="K10" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F10,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F10,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F10,256^0),256),8)</f>
         <v>000000001110000000000000</v>
       </c>
       <c r="L10" s="17" t="s">
@@ -1170,7 +1170,7 @@
         <v>000000010001111111111111</v>
       </c>
       <c r="K11" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F11,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F11,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F11,256^0),256),8)</f>
         <v>000000010000000000000000</v>
       </c>
       <c r="L11" s="17" t="s">
@@ -1213,7 +1213,7 @@
         <v>000000010011111111111111</v>
       </c>
       <c r="K12" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F12,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F12,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F12,256^0),256),8)</f>
         <v>000000010010000000000000</v>
       </c>
       <c r="L12" s="17" t="s">
@@ -1256,7 +1256,7 @@
         <v>000000010101111111111111</v>
       </c>
       <c r="K13" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F13,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F13,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F13,256^0),256),8)</f>
         <v>000000010100000000000000</v>
       </c>
       <c r="L13" s="17" t="s">
@@ -1299,7 +1299,7 @@
         <v>000000010111111111111111</v>
       </c>
       <c r="K14" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F14,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F14,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F14,256^0),256),8)</f>
         <v>000000010110000000000000</v>
       </c>
       <c r="L14" s="17" t="s">
@@ -1344,7 +1344,7 @@
         <v>000000011001111111111111</v>
       </c>
       <c r="K15" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F15,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F15,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F15,256^0),256),8)</f>
         <v>000000011000000000000000</v>
       </c>
       <c r="L15" s="17" t="s">
@@ -1389,7 +1389,7 @@
         <v>000000011011111111111111</v>
       </c>
       <c r="K16" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F16,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F16,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F16,256^0),256),8)</f>
         <v>000000011010000000000000</v>
       </c>
       <c r="L16" s="17" t="s">
@@ -1434,7 +1434,7 @@
         <v>000000011101111111111111</v>
       </c>
       <c r="K17" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F17,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F17,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F17,256^0),256),8)</f>
         <v>000000011100000000000000</v>
       </c>
       <c r="L17" s="17" t="s">
@@ -1479,7 +1479,7 @@
         <v>000000011111111111111111</v>
       </c>
       <c r="K18" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F18,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F18,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F18,256^0),256),8)</f>
         <v>000000011110000000000000</v>
       </c>
       <c r="L18" s="17" t="s">
@@ -1524,7 +1524,7 @@
         <v>000000100001111111111111</v>
       </c>
       <c r="K19" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F19,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F19,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F19,256^0),256),8)</f>
         <v>000000100000000000000000</v>
       </c>
       <c r="L19" s="17" t="s">
@@ -1566,7 +1566,7 @@
         <v>000000100011111111111111</v>
       </c>
       <c r="K20" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F20,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F20,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F20,256^0),256),8)</f>
         <v>000000100010000000000000</v>
       </c>
       <c r="L20" s="17" t="s">
@@ -1607,7 +1607,7 @@
         <v>000000100100111111111111</v>
       </c>
       <c r="K21" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F21,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F21,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F21,256^0),256),8)</f>
         <v>000000100100000000000000</v>
       </c>
       <c r="L21" s="17"/>
@@ -1648,7 +1648,7 @@
         <v>000000100101111111111111</v>
       </c>
       <c r="K22" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F22,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F22,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F22,256^0),256),8)</f>
         <v>000000100101000000000000</v>
       </c>
       <c r="L22" s="17" t="s">
@@ -1693,7 +1693,7 @@
         <v>000000100110000111111111</v>
       </c>
       <c r="K23" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F23,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F23,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F23,256^0),256),8)</f>
         <v>000000100110000000000000</v>
       </c>
       <c r="L23" s="24" t="s">
@@ -1734,7 +1734,7 @@
         <v>000000101000000111111111</v>
       </c>
       <c r="K24" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F24,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F24,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F24,256^0),256),8)</f>
         <v>000000100110001000000000</v>
       </c>
       <c r="L24" s="24"/>
@@ -1775,7 +1775,7 @@
         <v>000000101001000111111111</v>
       </c>
       <c r="K25" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F25,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F25,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F25,256^0),256),8)</f>
         <v>000000101000001000000000</v>
       </c>
       <c r="L25" s="17" t="s">
@@ -1818,7 +1818,7 @@
         <v>000000101010000111111111</v>
       </c>
       <c r="K26" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f>DEC2BIN(MOD(QUOTIENT($F26,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F26,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F26,256^0),256),8)</f>
         <v>000000101001001000000000</v>
       </c>
       <c r="L26" s="17" t="s">

</xml_diff>

<commit_message>
Fix MRA loading, update sys
</commit_message>
<xml_diff>
--- a/doc/rom_calc_tshoot.xlsx
+++ b/doc/rom_calc_tshoot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aberu\OneDrive\Documents\GitHub\Arcade-TurkeyShoot_MiSTer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587BAA46-4906-4A4E-95BB-9B83A7516550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E61ADCF-DA31-493E-B5E8-F85F83ED7C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
   <si>
     <t>MAME</t>
   </si>
@@ -121,9 +121,6 @@
     <t>rom21.ic58</t>
   </si>
   <si>
-    <t>BLANK</t>
-  </si>
-  <si>
     <t>turkey_shoot_bank_b</t>
   </si>
   <si>
@@ -277,9 +274,6 @@
     <t>1000</t>
   </si>
   <si>
-    <t>10100</t>
-  </si>
-  <si>
     <t>rom17.ic26</t>
   </si>
   <si>
@@ -292,10 +286,13 @@
     <t>421aafa8</t>
   </si>
   <si>
-    <t>100101</t>
-  </si>
-  <si>
-    <t>100110000</t>
+    <t>10010</t>
+  </si>
+  <si>
+    <t>100110</t>
+  </si>
+  <si>
+    <t>100111000</t>
   </si>
 </sst>
 </file>
@@ -427,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -475,9 +472,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -486,7 +480,17 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -708,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A4B22B-6618-4C49-8781-19881A3A2D30}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -790,13 +794,13 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>31</v>
-      </c>
       <c r="D3" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="15">
         <v>8192</v>
@@ -822,181 +826,181 @@
         <v>000000000001111111111111</v>
       </c>
       <c r="K3" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F3,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F3,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F3,256^0),256),8)</f>
+        <f t="shared" ref="K3:K24" si="0">DEC2BIN(MOD(QUOTIENT($F3,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F3,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F3,256^0),256),8)</f>
         <v>000000000000000000000000</v>
       </c>
       <c r="L3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="15">
         <v>8192</v>
       </c>
       <c r="F4" s="11">
-        <f t="shared" ref="F4:F26" si="0">E3+F3</f>
+        <f t="shared" ref="F4:F24" si="1">E3+F3</f>
         <v>8192</v>
       </c>
       <c r="G4" s="11">
-        <f t="shared" ref="G4:G26" si="1">E4+F4-1</f>
+        <f t="shared" ref="G4:G24" si="2">E4+F4-1</f>
         <v>16383</v>
       </c>
       <c r="H4" s="11" t="str">
-        <f t="shared" ref="H4:H26" si="2">DEC2HEX(E3+F3,5)</f>
+        <f t="shared" ref="H4:H24" si="3">DEC2HEX(E3+F3,5)</f>
         <v>02000</v>
       </c>
       <c r="I4" s="12" t="str">
-        <f t="shared" ref="I4:I26" si="3">DEC2HEX(E4+F4-1,5)</f>
+        <f t="shared" ref="I4:I24" si="4">DEC2HEX(E4+F4-1,5)</f>
         <v>03FFF</v>
       </c>
       <c r="J4" s="13" t="str">
-        <f t="shared" ref="J4:J26" si="4">DEC2BIN(MOD(QUOTIENT($G4,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($G4,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($G4,256^0),256),8)</f>
+        <f t="shared" ref="J4:J24" si="5">DEC2BIN(MOD(QUOTIENT($G4,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($G4,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($G4,256^0),256),8)</f>
         <v>000000000011111111111111</v>
       </c>
       <c r="K4" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F4,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F4,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F4,256^0),256),8)</f>
+        <f t="shared" si="0"/>
         <v>000000000010000000000000</v>
       </c>
       <c r="L4" s="14" t="s">
         <v>17</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="15">
         <v>8192</v>
       </c>
       <c r="F5" s="11">
+        <f t="shared" si="1"/>
+        <v>16384</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="2"/>
+        <v>24575</v>
+      </c>
+      <c r="H5" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>04000</v>
+      </c>
+      <c r="I5" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>05FFF</v>
+      </c>
+      <c r="J5" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000000101111111111111</v>
+      </c>
+      <c r="K5" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>16384</v>
-      </c>
-      <c r="G5" s="11">
-        <f t="shared" si="1"/>
-        <v>24575</v>
-      </c>
-      <c r="H5" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>04000</v>
-      </c>
-      <c r="I5" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>05FFF</v>
-      </c>
-      <c r="J5" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000000101111111111111</v>
-      </c>
-      <c r="K5" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F5,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F5,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F5,256^0),256),8)</f>
         <v>000000000100000000000000</v>
       </c>
       <c r="L5" s="14" t="s">
         <v>17</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="15">
         <v>8192</v>
       </c>
       <c r="F6" s="11">
+        <f t="shared" si="1"/>
+        <v>24576</v>
+      </c>
+      <c r="G6" s="11">
+        <f t="shared" si="2"/>
+        <v>32767</v>
+      </c>
+      <c r="H6" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>06000</v>
+      </c>
+      <c r="I6" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>07FFF</v>
+      </c>
+      <c r="J6" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000000111111111111111</v>
+      </c>
+      <c r="K6" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>24576</v>
-      </c>
-      <c r="G6" s="11">
-        <f t="shared" si="1"/>
-        <v>32767</v>
-      </c>
-      <c r="H6" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>06000</v>
-      </c>
-      <c r="I6" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>07FFF</v>
-      </c>
-      <c r="J6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000000111111111111111</v>
-      </c>
-      <c r="K6" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F6,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F6,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F6,256^0),256),8)</f>
         <v>000000000110000000000000</v>
       </c>
       <c r="L6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>36</v>
-      </c>
       <c r="D7" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="15">
         <v>8192</v>
       </c>
       <c r="F7" s="11">
+        <f t="shared" si="1"/>
+        <v>32768</v>
+      </c>
+      <c r="G7" s="11">
+        <f t="shared" si="2"/>
+        <v>40959</v>
+      </c>
+      <c r="H7" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>08000</v>
+      </c>
+      <c r="I7" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>09FFF</v>
+      </c>
+      <c r="J7" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000001001111111111111</v>
+      </c>
+      <c r="K7" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>32768</v>
-      </c>
-      <c r="G7" s="11">
-        <f t="shared" si="1"/>
-        <v>40959</v>
-      </c>
-      <c r="H7" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>08000</v>
-      </c>
-      <c r="I7" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>09FFF</v>
-      </c>
-      <c r="J7" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000001001111111111111</v>
-      </c>
-      <c r="K7" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F7,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F7,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F7,256^0),256),8)</f>
         <v>000000001000000000000000</v>
       </c>
       <c r="L7" s="17" t="s">
@@ -1010,36 +1014,36 @@
       <c r="A8" s="7"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="15">
         <v>8192</v>
       </c>
       <c r="F8" s="11">
+        <f t="shared" si="1"/>
+        <v>40960</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" si="2"/>
+        <v>49151</v>
+      </c>
+      <c r="H8" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0A000</v>
+      </c>
+      <c r="I8" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>0BFFF</v>
+      </c>
+      <c r="J8" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000001011111111111111</v>
+      </c>
+      <c r="K8" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>40960</v>
-      </c>
-      <c r="G8" s="11">
-        <f t="shared" si="1"/>
-        <v>49151</v>
-      </c>
-      <c r="H8" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>0A000</v>
-      </c>
-      <c r="I8" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>0BFFF</v>
-      </c>
-      <c r="J8" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000001011111111111111</v>
-      </c>
-      <c r="K8" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F8,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F8,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F8,256^0),256),8)</f>
         <v>000000001010000000000000</v>
       </c>
       <c r="L8" s="17" t="s">
@@ -1053,36 +1057,36 @@
       <c r="A9" s="7"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="15">
         <v>8192</v>
       </c>
       <c r="F9" s="11">
+        <f t="shared" si="1"/>
+        <v>49152</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="2"/>
+        <v>57343</v>
+      </c>
+      <c r="H9" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0C000</v>
+      </c>
+      <c r="I9" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>0DFFF</v>
+      </c>
+      <c r="J9" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000001101111111111111</v>
+      </c>
+      <c r="K9" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>49152</v>
-      </c>
-      <c r="G9" s="11">
-        <f t="shared" si="1"/>
-        <v>57343</v>
-      </c>
-      <c r="H9" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>0C000</v>
-      </c>
-      <c r="I9" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>0DFFF</v>
-      </c>
-      <c r="J9" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000001101111111111111</v>
-      </c>
-      <c r="K9" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F9,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F9,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F9,256^0),256),8)</f>
         <v>000000001100000000000000</v>
       </c>
       <c r="L9" s="17" t="s">
@@ -1096,36 +1100,36 @@
       <c r="A10" s="7"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="15">
         <v>8192</v>
       </c>
       <c r="F10" s="11">
+        <f t="shared" si="1"/>
+        <v>57344</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="2"/>
+        <v>65535</v>
+      </c>
+      <c r="H10" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>0E000</v>
+      </c>
+      <c r="I10" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>0FFFF</v>
+      </c>
+      <c r="J10" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000001111111111111111</v>
+      </c>
+      <c r="K10" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>57344</v>
-      </c>
-      <c r="G10" s="11">
-        <f t="shared" si="1"/>
-        <v>65535</v>
-      </c>
-      <c r="H10" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>0E000</v>
-      </c>
-      <c r="I10" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>0FFFF</v>
-      </c>
-      <c r="J10" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000001111111111111111</v>
-      </c>
-      <c r="K10" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F10,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F10,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F10,256^0),256),8)</f>
         <v>000000001110000000000000</v>
       </c>
       <c r="L10" s="17" t="s">
@@ -1138,39 +1142,39 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>41</v>
-      </c>
       <c r="D11" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" s="15">
         <v>8192</v>
       </c>
       <c r="F11" s="11">
+        <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="G11" s="11">
+        <f t="shared" si="2"/>
+        <v>73727</v>
+      </c>
+      <c r="H11" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>10000</v>
+      </c>
+      <c r="I11" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>11FFF</v>
+      </c>
+      <c r="J11" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000010001111111111111</v>
+      </c>
+      <c r="K11" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>65536</v>
-      </c>
-      <c r="G11" s="11">
-        <f t="shared" si="1"/>
-        <v>73727</v>
-      </c>
-      <c r="H11" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>10000</v>
-      </c>
-      <c r="I11" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>11FFF</v>
-      </c>
-      <c r="J11" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000010001111111111111</v>
-      </c>
-      <c r="K11" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F11,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F11,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F11,256^0),256),8)</f>
         <v>000000010000000000000000</v>
       </c>
       <c r="L11" s="17" t="s">
@@ -1184,36 +1188,36 @@
       <c r="A12" s="7"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="15">
         <v>8192</v>
       </c>
       <c r="F12" s="11">
+        <f t="shared" si="1"/>
+        <v>73728</v>
+      </c>
+      <c r="G12" s="11">
+        <f t="shared" si="2"/>
+        <v>81919</v>
+      </c>
+      <c r="H12" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>12000</v>
+      </c>
+      <c r="I12" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>13FFF</v>
+      </c>
+      <c r="J12" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000010011111111111111</v>
+      </c>
+      <c r="K12" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>73728</v>
-      </c>
-      <c r="G12" s="11">
-        <f t="shared" si="1"/>
-        <v>81919</v>
-      </c>
-      <c r="H12" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>12000</v>
-      </c>
-      <c r="I12" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>13FFF</v>
-      </c>
-      <c r="J12" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000010011111111111111</v>
-      </c>
-      <c r="K12" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F12,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F12,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F12,256^0),256),8)</f>
         <v>000000010010000000000000</v>
       </c>
       <c r="L12" s="17" t="s">
@@ -1227,36 +1231,36 @@
       <c r="A13" s="7"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="15">
         <v>8192</v>
       </c>
       <c r="F13" s="11">
+        <f t="shared" si="1"/>
+        <v>81920</v>
+      </c>
+      <c r="G13" s="11">
+        <f t="shared" si="2"/>
+        <v>90111</v>
+      </c>
+      <c r="H13" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>14000</v>
+      </c>
+      <c r="I13" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>15FFF</v>
+      </c>
+      <c r="J13" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000010101111111111111</v>
+      </c>
+      <c r="K13" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>81920</v>
-      </c>
-      <c r="G13" s="11">
-        <f t="shared" si="1"/>
-        <v>90111</v>
-      </c>
-      <c r="H13" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>14000</v>
-      </c>
-      <c r="I13" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>15FFF</v>
-      </c>
-      <c r="J13" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000010101111111111111</v>
-      </c>
-      <c r="K13" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F13,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F13,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F13,256^0),256),8)</f>
         <v>000000010100000000000000</v>
       </c>
       <c r="L13" s="17" t="s">
@@ -1270,36 +1274,36 @@
       <c r="A14" s="7"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="15">
         <v>8192</v>
       </c>
       <c r="F14" s="11">
+        <f t="shared" si="1"/>
+        <v>90112</v>
+      </c>
+      <c r="G14" s="11">
+        <f t="shared" si="2"/>
+        <v>98303</v>
+      </c>
+      <c r="H14" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>16000</v>
+      </c>
+      <c r="I14" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>17FFF</v>
+      </c>
+      <c r="J14" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000010111111111111111</v>
+      </c>
+      <c r="K14" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>90112</v>
-      </c>
-      <c r="G14" s="11">
-        <f t="shared" si="1"/>
-        <v>98303</v>
-      </c>
-      <c r="H14" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>16000</v>
-      </c>
-      <c r="I14" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>17FFF</v>
-      </c>
-      <c r="J14" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000010111111111111111</v>
-      </c>
-      <c r="K14" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F14,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F14,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F14,256^0),256),8)</f>
         <v>000000010110000000000000</v>
       </c>
       <c r="L14" s="17" t="s">
@@ -1318,40 +1322,40 @@
         <v>27</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" s="15">
         <v>8192</v>
       </c>
       <c r="F15" s="11">
+        <f t="shared" si="1"/>
+        <v>98304</v>
+      </c>
+      <c r="G15" s="11">
+        <f t="shared" si="2"/>
+        <v>106495</v>
+      </c>
+      <c r="H15" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>18000</v>
+      </c>
+      <c r="I15" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>19FFF</v>
+      </c>
+      <c r="J15" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000011001111111111111</v>
+      </c>
+      <c r="K15" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>98304</v>
-      </c>
-      <c r="G15" s="11">
-        <f t="shared" si="1"/>
-        <v>106495</v>
-      </c>
-      <c r="H15" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>18000</v>
-      </c>
-      <c r="I15" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>19FFF</v>
-      </c>
-      <c r="J15" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000011001111111111111</v>
-      </c>
-      <c r="K15" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F15,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F15,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F15,256^0),256),8)</f>
         <v>000000011000000000000000</v>
       </c>
       <c r="L15" s="17" t="s">
         <v>16</v>
       </c>
       <c r="M15" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1363,40 +1367,40 @@
         <v>28</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" s="15">
         <v>8192</v>
       </c>
       <c r="F16" s="11">
+        <f t="shared" si="1"/>
+        <v>106496</v>
+      </c>
+      <c r="G16" s="11">
+        <f t="shared" si="2"/>
+        <v>114687</v>
+      </c>
+      <c r="H16" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1A000</v>
+      </c>
+      <c r="I16" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>1BFFF</v>
+      </c>
+      <c r="J16" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000011011111111111111</v>
+      </c>
+      <c r="K16" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>106496</v>
-      </c>
-      <c r="G16" s="11">
-        <f t="shared" si="1"/>
-        <v>114687</v>
-      </c>
-      <c r="H16" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>1A000</v>
-      </c>
-      <c r="I16" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>1BFFF</v>
-      </c>
-      <c r="J16" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000011011111111111111</v>
-      </c>
-      <c r="K16" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F16,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F16,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F16,256^0),256),8)</f>
         <v>000000011010000000000000</v>
       </c>
       <c r="L16" s="17" t="s">
         <v>16</v>
       </c>
       <c r="M16" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1408,40 +1412,40 @@
         <v>22</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E17" s="15">
         <v>8192</v>
       </c>
       <c r="F17" s="11">
+        <f t="shared" si="1"/>
+        <v>114688</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="2"/>
+        <v>122879</v>
+      </c>
+      <c r="H17" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1C000</v>
+      </c>
+      <c r="I17" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>1DFFF</v>
+      </c>
+      <c r="J17" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000011101111111111111</v>
+      </c>
+      <c r="K17" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>114688</v>
-      </c>
-      <c r="G17" s="11">
-        <f t="shared" si="1"/>
-        <v>122879</v>
-      </c>
-      <c r="H17" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>1C000</v>
-      </c>
-      <c r="I17" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>1DFFF</v>
-      </c>
-      <c r="J17" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000011101111111111111</v>
-      </c>
-      <c r="K17" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F17,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F17,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F17,256^0),256),8)</f>
         <v>000000011100000000000000</v>
       </c>
       <c r="L17" s="17" t="s">
         <v>16</v>
       </c>
       <c r="M17" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1453,380 +1457,316 @@
         <v>24</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" s="15">
         <v>8192</v>
       </c>
       <c r="F18" s="11">
+        <f t="shared" si="1"/>
+        <v>122880</v>
+      </c>
+      <c r="G18" s="11">
+        <f t="shared" si="2"/>
+        <v>131071</v>
+      </c>
+      <c r="H18" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>1E000</v>
+      </c>
+      <c r="I18" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>1FFFF</v>
+      </c>
+      <c r="J18" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000011111111111111111</v>
+      </c>
+      <c r="K18" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>122880</v>
-      </c>
-      <c r="G18" s="11">
-        <f t="shared" si="1"/>
-        <v>131071</v>
-      </c>
-      <c r="H18" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>1E000</v>
-      </c>
-      <c r="I18" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>1FFFF</v>
-      </c>
-      <c r="J18" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000011111111111111111</v>
-      </c>
-      <c r="K18" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F18,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F18,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F18,256^0),256),8)</f>
         <v>000000011110000000000000</v>
       </c>
       <c r="L18" s="17" t="s">
         <v>16</v>
       </c>
       <c r="M18" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="E19" s="15">
         <v>8192</v>
       </c>
       <c r="F19" s="11">
+        <f t="shared" si="1"/>
+        <v>131072</v>
+      </c>
+      <c r="G19" s="11">
+        <f t="shared" si="2"/>
+        <v>139263</v>
+      </c>
+      <c r="H19" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="I19" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>21FFF</v>
+      </c>
+      <c r="J19" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000100001111111111111</v>
+      </c>
+      <c r="K19" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>131072</v>
-      </c>
-      <c r="G19" s="11">
-        <f t="shared" si="1"/>
-        <v>139263</v>
-      </c>
-      <c r="H19" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>20000</v>
-      </c>
-      <c r="I19" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>21FFF</v>
-      </c>
-      <c r="J19" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000100001111111111111</v>
-      </c>
-      <c r="K19" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F19,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F19,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F19,256^0),256),8)</f>
         <v>000000100000000000000000</v>
       </c>
       <c r="L19" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="M19" s="20" t="s">
         <v>79</v>
-      </c>
-      <c r="M19" s="20" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="C20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E20" s="15">
         <v>8192</v>
       </c>
       <c r="F20" s="11">
+        <f t="shared" si="1"/>
+        <v>139264</v>
+      </c>
+      <c r="G20" s="11">
+        <f t="shared" si="2"/>
+        <v>147455</v>
+      </c>
+      <c r="H20" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>22000</v>
+      </c>
+      <c r="I20" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>23FFF</v>
+      </c>
+      <c r="J20" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000100011111111111111</v>
+      </c>
+      <c r="K20" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>139264</v>
-      </c>
-      <c r="G20" s="11">
-        <f t="shared" si="1"/>
-        <v>147455</v>
-      </c>
-      <c r="H20" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>22000</v>
-      </c>
-      <c r="I20" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>23FFF</v>
-      </c>
-      <c r="J20" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000100011111111111111</v>
-      </c>
-      <c r="K20" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F20,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F20,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F20,256^0),256),8)</f>
         <v>000000100010000000000000</v>
       </c>
       <c r="L20" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="M20" s="20" t="s">
         <v>79</v>
-      </c>
-      <c r="M20" s="20" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
+        <v>63</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="E21" s="15">
         <v>4096</v>
       </c>
       <c r="F21" s="11">
+        <f t="shared" si="1"/>
+        <v>147456</v>
+      </c>
+      <c r="G21" s="11">
+        <f t="shared" si="2"/>
+        <v>151551</v>
+      </c>
+      <c r="H21" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>24000</v>
+      </c>
+      <c r="I21" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>24FFF</v>
+      </c>
+      <c r="J21" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000100100111111111111</v>
+      </c>
+      <c r="K21" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>147456</v>
-      </c>
-      <c r="G21" s="11">
-        <f t="shared" si="1"/>
-        <v>151551</v>
-      </c>
-      <c r="H21" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>24000</v>
-      </c>
-      <c r="I21" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>24FFF</v>
-      </c>
-      <c r="J21" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000100100111111111111</v>
-      </c>
-      <c r="K21" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F21,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F21,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F21,256^0),256),8)</f>
         <v>000000100100000000000000</v>
       </c>
-      <c r="L21" s="17"/>
-      <c r="M21" s="20"/>
+      <c r="L21" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="M21" s="20" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="22" t="s">
-        <v>46</v>
-      </c>
+      <c r="B22" s="22"/>
       <c r="C22" s="22" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E22" s="15">
         <v>4096</v>
       </c>
       <c r="F22" s="11">
+        <f t="shared" si="1"/>
+        <v>151552</v>
+      </c>
+      <c r="G22" s="11">
+        <f t="shared" si="2"/>
+        <v>155647</v>
+      </c>
+      <c r="H22" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>25000</v>
+      </c>
+      <c r="I22" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>25FFF</v>
+      </c>
+      <c r="J22" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000100101111111111111</v>
+      </c>
+      <c r="K22" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>151552</v>
-      </c>
-      <c r="G22" s="11">
-        <f t="shared" si="1"/>
-        <v>155647</v>
-      </c>
-      <c r="H22" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>25000</v>
-      </c>
-      <c r="I22" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>25FFF</v>
-      </c>
-      <c r="J22" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000100101111111111111</v>
-      </c>
-      <c r="K22" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F22,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F22,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F22,256^0),256),8)</f>
         <v>000000100101000000000000</v>
       </c>
-      <c r="L22" s="17" t="s">
-        <v>67</v>
-      </c>
+      <c r="L22" s="17"/>
       <c r="M22" s="20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="22" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E23" s="15">
-        <v>512</v>
+        <v>4096</v>
       </c>
       <c r="F23" s="11">
+        <f t="shared" si="1"/>
+        <v>155648</v>
+      </c>
+      <c r="G23" s="11">
+        <f t="shared" si="2"/>
+        <v>159743</v>
+      </c>
+      <c r="H23" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>26000</v>
+      </c>
+      <c r="I23" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>26FFF</v>
+      </c>
+      <c r="J23" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000100110111111111111</v>
+      </c>
+      <c r="K23" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>155648</v>
-      </c>
-      <c r="G23" s="11">
-        <f t="shared" si="1"/>
-        <v>156159</v>
-      </c>
-      <c r="H23" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>26000</v>
-      </c>
-      <c r="I23" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>261FF</v>
-      </c>
-      <c r="J23" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000100110000111111111</v>
-      </c>
-      <c r="K23" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F23,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F23,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F23,256^0),256),8)</f>
         <v>000000100110000000000000</v>
       </c>
-      <c r="L23" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="M23" s="24" t="s">
-        <v>87</v>
+      <c r="L23" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="M23" s="23" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="15">
-        <v>8192</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="15"/>
       <c r="F24" s="11">
+        <f t="shared" si="1"/>
+        <v>159744</v>
+      </c>
+      <c r="G24" s="11">
+        <f t="shared" si="2"/>
+        <v>159743</v>
+      </c>
+      <c r="H24" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>27000</v>
+      </c>
+      <c r="I24" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v>26FFF</v>
+      </c>
+      <c r="J24" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>000000100110111111111111</v>
+      </c>
+      <c r="K24" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>156160</v>
-      </c>
-      <c r="G24" s="11">
-        <f t="shared" si="1"/>
-        <v>164351</v>
-      </c>
-      <c r="H24" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>26200</v>
-      </c>
-      <c r="I24" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>281FF</v>
-      </c>
-      <c r="J24" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000101000000111111111</v>
-      </c>
-      <c r="K24" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F24,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F24,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F24,256^0),256),8)</f>
-        <v>000000100110001000000000</v>
-      </c>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="15">
-        <v>4096</v>
-      </c>
-      <c r="F25" s="11">
-        <f t="shared" si="0"/>
-        <v>164352</v>
-      </c>
-      <c r="G25" s="11">
-        <f t="shared" si="1"/>
-        <v>168447</v>
-      </c>
-      <c r="H25" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>28200</v>
-      </c>
-      <c r="I25" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>291FF</v>
-      </c>
-      <c r="J25" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000101001000111111111</v>
-      </c>
-      <c r="K25" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F25,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F25,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F25,256^0),256),8)</f>
-        <v>000000101000001000000000</v>
-      </c>
-      <c r="L25" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="M25" s="20" t="s">
-        <v>81</v>
+        <v>000000100111000000000000</v>
+      </c>
+      <c r="L24" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24" s="23" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E26" s="15">
-        <v>4096</v>
-      </c>
-      <c r="F26" s="11">
-        <f t="shared" si="0"/>
-        <v>168448</v>
-      </c>
-      <c r="G26" s="11">
-        <f t="shared" si="1"/>
-        <v>172543</v>
-      </c>
-      <c r="H26" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>29200</v>
-      </c>
-      <c r="I26" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>2A1FF</v>
-      </c>
-      <c r="J26" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>000000101010000111111111</v>
-      </c>
-      <c r="K26" s="13" t="str">
-        <f>DEC2BIN(MOD(QUOTIENT($F26,256^2),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F26,256^1),256),8)&amp;DEC2BIN(MOD(QUOTIENT($F26,256^0),256),8)</f>
-        <v>000000101001001000000000</v>
-      </c>
-      <c r="L26" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="M26" s="20" t="s">
-        <v>81</v>
-      </c>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="9"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
@@ -1849,23 +1789,12 @@
       <c r="D30" s="21"/>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="9"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D22:D23 D7:D18 D25">
-    <cfRule type="duplicateValues" dxfId="0" priority="31"/>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:D18 D23:D24">
+    <cfRule type="duplicateValues" dxfId="0" priority="34"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>